<commit_message>
enhanced everything is upto date
</commit_message>
<xml_diff>
--- a/Macro_Functional_Excel.xlsx
+++ b/Macro_Functional_Excel.xlsx
@@ -62,7 +62,7 @@
     <t>000003- AZ (PPO)- H5521 (PBP) 200</t>
   </si>
   <si>
-    <t>Group. medicate (V01)_- ESA (PPO)-Local 147 -Construction-WorkersFund</t>
+    <t>Group. medicare (V01)_- ESA (PPO)-Local 147 -Construction-WorkersFund</t>
   </si>
   <si>
     <t>Group_-Medicare (SO3) (HMO)_-District-Council33_-Medicare</t>
@@ -80,25 +80,20 @@
     <t>000043 (EX) - STATECODE Plantype34_-Details</t>
   </si>
   <si>
-    <t>Group.Medicare (SO3) (HMO) Distict-Council33_-Medicare</t>
+    <t>Group.Medicare (SO3) (HMO) Distict-Council33</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -110,31 +105,13 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left>
-        <color indexed="64"/>
-      </left>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top>
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-      <diagonal>
-        <color indexed="64"/>
-      </diagonal>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -475,7 +452,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -507,66 +484,66 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" ht="30">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>